<commit_message>
Actualizacion Carpeta Documentacion 9
</commit_message>
<xml_diff>
--- a/Documentacion/Backlog ,Sprints, Story Mapping/6.0Backlog, Sprints, Story Mapping.xlsx
+++ b/Documentacion/Backlog ,Sprints, Story Mapping/6.0Backlog, Sprints, Story Mapping.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juane\OneDrive - unicauca.edu.co\Desktop\Proyecto-Software-I\Documentacion\Backlog ,Sprints, Story Mapping\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcben\OneDrive\Escritorio\Proyecto-Software-I\Documentacion\Backlog ,Sprints, Story Mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F750DFE-8FCE-4E76-A2E9-8EBF86C5B874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFE6F275-E122-41B6-B35A-372ED19BD460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog de producto x Epicas" sheetId="1" r:id="rId1"/>
@@ -721,27 +721,27 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -998,7 +998,9 @@
   </sheetPr>
   <dimension ref="D5:P24"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="H12" zoomScale="86" workbookViewId="0">
+      <selection activeCell="S15" sqref="S15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -1148,7 +1150,7 @@
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
     </row>
-    <row r="13" spans="4:16" ht="72">
+    <row r="13" spans="4:16" ht="57.6">
       <c r="D13" s="5">
         <v>3</v>
       </c>
@@ -1164,20 +1166,20 @@
       <c r="H13" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="L13" s="5">
+      <c r="L13" s="1">
         <v>3</v>
       </c>
-      <c r="M13" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="N13" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="O13" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="P13" s="6" t="s">
-        <v>14</v>
+      <c r="M13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="P13" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="4:16" ht="14.4">
@@ -1208,20 +1210,20 @@
       <c r="H15" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L15" s="1">
+      <c r="L15" s="5">
         <v>4</v>
       </c>
-      <c r="M15" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="N15" s="2" t="s">
+      <c r="M15" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="N15" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="O15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="P15" s="2" t="s">
-        <v>11</v>
+      <c r="O15" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="P15" s="6" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="4:16" ht="12.75" customHeight="1">
@@ -1256,16 +1258,16 @@
         <v>5</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="N17" s="2" t="s">
         <v>3</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="4:16" ht="15" customHeight="1">
@@ -1300,16 +1302,16 @@
         <v>6</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="O19" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="4:16" ht="15" customHeight="1">
@@ -1660,16 +1662,16 @@
       <c r="D33" s="46">
         <v>8</v>
       </c>
-      <c r="E33" s="47" t="s">
+      <c r="E33" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="F33" s="47" t="s">
+      <c r="F33" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="G33" s="47" t="s">
+      <c r="G33" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="H33" s="47" t="s">
+      <c r="H33" s="50" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1834,11 +1836,11 @@
     </row>
     <row r="51" spans="4:16" ht="18" customHeight="1"/>
     <row r="53" spans="4:16" ht="18" customHeight="1">
-      <c r="J53" s="52"/>
-      <c r="K53" s="52"/>
-      <c r="L53" s="52"/>
-      <c r="M53" s="52"/>
-      <c r="N53" s="52"/>
+      <c r="J53" s="49"/>
+      <c r="K53" s="49"/>
+      <c r="L53" s="49"/>
+      <c r="M53" s="49"/>
+      <c r="N53" s="49"/>
     </row>
     <row r="54" spans="4:16" ht="18" customHeight="1">
       <c r="D54" s="11"/>
@@ -1877,7 +1879,7 @@
       <c r="H56" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="J56" s="49" t="s">
+      <c r="J56" s="48" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1906,7 +1908,7 @@
       <c r="J59" s="15"/>
     </row>
     <row r="60" spans="4:16" ht="18" customHeight="1">
-      <c r="D60" s="50">
+      <c r="D60" s="47">
         <v>2</v>
       </c>
       <c r="E60" s="42" t="s">
@@ -1921,7 +1923,7 @@
       <c r="H60" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="J60" s="49" t="s">
+      <c r="J60" s="48" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1958,7 +1960,7 @@
       <c r="J64" s="18"/>
     </row>
     <row r="65" spans="4:10" ht="18" customHeight="1">
-      <c r="D65" s="50">
+      <c r="D65" s="47">
         <v>3</v>
       </c>
       <c r="E65" s="42" t="s">
@@ -1973,7 +1975,7 @@
       <c r="H65" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="J65" s="49" t="s">
+      <c r="J65" s="48" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2002,7 +2004,7 @@
       <c r="J68" s="19"/>
     </row>
     <row r="69" spans="4:10" ht="18" customHeight="1">
-      <c r="D69" s="50">
+      <c r="D69" s="47">
         <v>4</v>
       </c>
       <c r="E69" s="42" t="s">
@@ -2011,13 +2013,13 @@
       <c r="F69" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="G69" s="48" t="s">
+      <c r="G69" s="54" t="s">
         <v>45</v>
       </c>
       <c r="H69" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="J69" s="49" t="s">
+      <c r="J69" s="48" t="s">
         <v>65</v>
       </c>
     </row>
@@ -2054,7 +2056,7 @@
       <c r="J73" s="20"/>
     </row>
     <row r="74" spans="4:10" ht="13.8">
-      <c r="D74" s="50">
+      <c r="D74" s="47">
         <v>5</v>
       </c>
       <c r="E74" s="42" t="s">
@@ -2066,10 +2068,10 @@
       <c r="G74" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="H74" s="48" t="s">
+      <c r="H74" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="J74" s="49" t="s">
+      <c r="J74" s="48" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2162,7 +2164,7 @@
       <c r="J82" s="18"/>
     </row>
     <row r="83" spans="4:10" ht="41.25" customHeight="1">
-      <c r="D83" s="50">
+      <c r="D83" s="47">
         <v>8</v>
       </c>
       <c r="E83" s="42" t="s">
@@ -2171,13 +2173,13 @@
       <c r="F83" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="G83" s="48" t="s">
+      <c r="G83" s="54" t="s">
         <v>38</v>
       </c>
       <c r="H83" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="J83" s="49" t="s">
+      <c r="J83" s="48" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2198,22 +2200,22 @@
       <c r="J85" s="18"/>
     </row>
     <row r="86" spans="4:10" ht="18" customHeight="1">
-      <c r="D86" s="50">
+      <c r="D86" s="47">
         <v>9</v>
       </c>
-      <c r="E86" s="47" t="s">
+      <c r="E86" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="F86" s="47" t="s">
+      <c r="F86" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="G86" s="47" t="s">
+      <c r="G86" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="H86" s="47" t="s">
+      <c r="H86" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="J86" s="49" t="s">
+      <c r="J86" s="48" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2270,7 +2272,7 @@
       <c r="J91" s="18"/>
     </row>
     <row r="92" spans="4:10" ht="18" customHeight="1">
-      <c r="D92" s="50">
+      <c r="D92" s="47">
         <v>11</v>
       </c>
       <c r="E92" s="42" t="s">
@@ -2285,7 +2287,7 @@
       <c r="H92" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="J92" s="49" t="s">
+      <c r="J92" s="48" t="s">
         <v>75</v>
       </c>
     </row>
@@ -2322,7 +2324,7 @@
       <c r="J96" s="15"/>
     </row>
     <row r="97" spans="4:13" ht="18" customHeight="1">
-      <c r="D97" s="50">
+      <c r="D97" s="47">
         <v>12</v>
       </c>
       <c r="E97" s="42" t="s">
@@ -2337,7 +2339,7 @@
       <c r="H97" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="J97" s="49" t="s">
+      <c r="J97" s="48" t="s">
         <v>76</v>
       </c>
     </row>
@@ -2375,27 +2377,27 @@
     </row>
     <row r="102" spans="4:13" ht="18" customHeight="1">
       <c r="D102" s="51"/>
-      <c r="E102" s="53"/>
-      <c r="F102" s="53"/>
-      <c r="G102" s="53"/>
-      <c r="H102" s="53"/>
-      <c r="J102" s="54"/>
+      <c r="E102" s="52"/>
+      <c r="F102" s="52"/>
+      <c r="G102" s="52"/>
+      <c r="H102" s="52"/>
+      <c r="J102" s="53"/>
     </row>
     <row r="103" spans="4:13" ht="18" customHeight="1">
-      <c r="D103" s="52"/>
-      <c r="E103" s="52"/>
-      <c r="F103" s="52"/>
-      <c r="G103" s="52"/>
-      <c r="H103" s="52"/>
-      <c r="J103" s="52"/>
+      <c r="D103" s="49"/>
+      <c r="E103" s="49"/>
+      <c r="F103" s="49"/>
+      <c r="G103" s="49"/>
+      <c r="H103" s="49"/>
+      <c r="J103" s="49"/>
     </row>
     <row r="104" spans="4:13" ht="18" customHeight="1">
-      <c r="D104" s="52"/>
-      <c r="E104" s="52"/>
-      <c r="F104" s="52"/>
-      <c r="G104" s="52"/>
-      <c r="H104" s="52"/>
-      <c r="J104" s="52"/>
+      <c r="D104" s="49"/>
+      <c r="E104" s="49"/>
+      <c r="F104" s="49"/>
+      <c r="G104" s="49"/>
+      <c r="H104" s="49"/>
+      <c r="J104" s="49"/>
       <c r="M104" s="26"/>
     </row>
     <row r="105" spans="4:13" ht="18" customHeight="1"/>
@@ -3298,73 +3300,32 @@
     <row r="1002" ht="18" customHeight="1"/>
   </sheetData>
   <mergeCells count="113">
-    <mergeCell ref="D65:D67"/>
-    <mergeCell ref="E65:E67"/>
-    <mergeCell ref="F65:F67"/>
-    <mergeCell ref="G65:G67"/>
-    <mergeCell ref="H65:H67"/>
-    <mergeCell ref="J65:J67"/>
-    <mergeCell ref="D69:D72"/>
-    <mergeCell ref="J69:J72"/>
-    <mergeCell ref="E92:E95"/>
-    <mergeCell ref="F92:F95"/>
-    <mergeCell ref="J53:N53"/>
-    <mergeCell ref="D55:H55"/>
-    <mergeCell ref="E56:E58"/>
-    <mergeCell ref="F56:F58"/>
-    <mergeCell ref="G56:G58"/>
-    <mergeCell ref="H56:H58"/>
-    <mergeCell ref="J56:J58"/>
-    <mergeCell ref="D56:D58"/>
-    <mergeCell ref="D60:D63"/>
-    <mergeCell ref="E60:E63"/>
-    <mergeCell ref="F60:F63"/>
-    <mergeCell ref="G60:G63"/>
-    <mergeCell ref="H60:H63"/>
-    <mergeCell ref="J60:J63"/>
-    <mergeCell ref="D28:D31"/>
-    <mergeCell ref="E28:E31"/>
-    <mergeCell ref="F28:F31"/>
-    <mergeCell ref="G28:G31"/>
-    <mergeCell ref="H28:H31"/>
-    <mergeCell ref="D33:D35"/>
-    <mergeCell ref="E33:E35"/>
-    <mergeCell ref="F33:F35"/>
-    <mergeCell ref="D39:D41"/>
-    <mergeCell ref="E39:E41"/>
-    <mergeCell ref="F39:F41"/>
-    <mergeCell ref="G39:G41"/>
-    <mergeCell ref="H39:H41"/>
-    <mergeCell ref="D102:D104"/>
-    <mergeCell ref="E102:E104"/>
-    <mergeCell ref="F102:F104"/>
-    <mergeCell ref="G102:G104"/>
-    <mergeCell ref="H102:H104"/>
-    <mergeCell ref="J102:J104"/>
-    <mergeCell ref="D92:D95"/>
-    <mergeCell ref="D97:D100"/>
-    <mergeCell ref="E97:E100"/>
-    <mergeCell ref="F97:F100"/>
-    <mergeCell ref="G97:G100"/>
-    <mergeCell ref="H97:H100"/>
-    <mergeCell ref="J97:J100"/>
-    <mergeCell ref="G92:G95"/>
-    <mergeCell ref="H92:H95"/>
-    <mergeCell ref="D86:D88"/>
-    <mergeCell ref="E86:E88"/>
-    <mergeCell ref="F86:F88"/>
-    <mergeCell ref="G86:G88"/>
-    <mergeCell ref="H86:H88"/>
-    <mergeCell ref="J86:J88"/>
-    <mergeCell ref="J92:J95"/>
-    <mergeCell ref="E69:E72"/>
-    <mergeCell ref="F69:F72"/>
-    <mergeCell ref="E74:E77"/>
-    <mergeCell ref="F74:F77"/>
-    <mergeCell ref="G74:G77"/>
-    <mergeCell ref="H74:H77"/>
-    <mergeCell ref="J74:J77"/>
-    <mergeCell ref="D74:D77"/>
+    <mergeCell ref="G9:G12"/>
+    <mergeCell ref="H9:H12"/>
+    <mergeCell ref="D3:H3"/>
+    <mergeCell ref="D4:D7"/>
+    <mergeCell ref="E4:E7"/>
+    <mergeCell ref="F4:F7"/>
+    <mergeCell ref="G4:G7"/>
+    <mergeCell ref="H4:H7"/>
+    <mergeCell ref="D9:D12"/>
+    <mergeCell ref="E9:E12"/>
+    <mergeCell ref="F9:F12"/>
+    <mergeCell ref="D16:D19"/>
+    <mergeCell ref="E16:E19"/>
+    <mergeCell ref="F16:F19"/>
+    <mergeCell ref="G16:G19"/>
+    <mergeCell ref="H16:H19"/>
+    <mergeCell ref="F24:F26"/>
+    <mergeCell ref="G24:G26"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="H21:H22"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="H24:H26"/>
+    <mergeCell ref="D24:D26"/>
     <mergeCell ref="D83:D84"/>
     <mergeCell ref="E83:E84"/>
     <mergeCell ref="F83:F84"/>
@@ -3385,32 +3346,73 @@
     <mergeCell ref="D47:D49"/>
     <mergeCell ref="E47:E49"/>
     <mergeCell ref="H47:H49"/>
-    <mergeCell ref="D16:D19"/>
-    <mergeCell ref="E16:E19"/>
-    <mergeCell ref="F16:F19"/>
-    <mergeCell ref="G16:G19"/>
-    <mergeCell ref="H16:H19"/>
-    <mergeCell ref="F24:F26"/>
-    <mergeCell ref="G24:G26"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="H21:H22"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="H24:H26"/>
-    <mergeCell ref="D24:D26"/>
-    <mergeCell ref="G9:G12"/>
-    <mergeCell ref="H9:H12"/>
-    <mergeCell ref="D3:H3"/>
-    <mergeCell ref="D4:D7"/>
-    <mergeCell ref="E4:E7"/>
-    <mergeCell ref="F4:F7"/>
-    <mergeCell ref="G4:G7"/>
-    <mergeCell ref="H4:H7"/>
-    <mergeCell ref="D9:D12"/>
-    <mergeCell ref="E9:E12"/>
-    <mergeCell ref="F9:F12"/>
+    <mergeCell ref="D102:D104"/>
+    <mergeCell ref="E102:E104"/>
+    <mergeCell ref="F102:F104"/>
+    <mergeCell ref="G102:G104"/>
+    <mergeCell ref="H102:H104"/>
+    <mergeCell ref="J102:J104"/>
+    <mergeCell ref="D92:D95"/>
+    <mergeCell ref="D97:D100"/>
+    <mergeCell ref="E97:E100"/>
+    <mergeCell ref="F97:F100"/>
+    <mergeCell ref="G97:G100"/>
+    <mergeCell ref="H97:H100"/>
+    <mergeCell ref="J97:J100"/>
+    <mergeCell ref="G92:G95"/>
+    <mergeCell ref="H92:H95"/>
+    <mergeCell ref="J92:J95"/>
+    <mergeCell ref="D28:D31"/>
+    <mergeCell ref="E28:E31"/>
+    <mergeCell ref="F28:F31"/>
+    <mergeCell ref="G28:G31"/>
+    <mergeCell ref="H28:H31"/>
+    <mergeCell ref="D33:D35"/>
+    <mergeCell ref="E33:E35"/>
+    <mergeCell ref="F33:F35"/>
+    <mergeCell ref="D39:D41"/>
+    <mergeCell ref="E39:E41"/>
+    <mergeCell ref="F39:F41"/>
+    <mergeCell ref="G39:G41"/>
+    <mergeCell ref="H39:H41"/>
+    <mergeCell ref="J53:N53"/>
+    <mergeCell ref="D55:H55"/>
+    <mergeCell ref="E56:E58"/>
+    <mergeCell ref="F56:F58"/>
+    <mergeCell ref="G56:G58"/>
+    <mergeCell ref="H56:H58"/>
+    <mergeCell ref="J56:J58"/>
+    <mergeCell ref="D56:D58"/>
+    <mergeCell ref="D60:D63"/>
+    <mergeCell ref="E60:E63"/>
+    <mergeCell ref="F60:F63"/>
+    <mergeCell ref="G60:G63"/>
+    <mergeCell ref="H60:H63"/>
+    <mergeCell ref="J60:J63"/>
+    <mergeCell ref="D65:D67"/>
+    <mergeCell ref="E65:E67"/>
+    <mergeCell ref="F65:F67"/>
+    <mergeCell ref="G65:G67"/>
+    <mergeCell ref="H65:H67"/>
+    <mergeCell ref="J65:J67"/>
+    <mergeCell ref="D69:D72"/>
+    <mergeCell ref="J69:J72"/>
+    <mergeCell ref="E92:E95"/>
+    <mergeCell ref="F92:F95"/>
+    <mergeCell ref="D86:D88"/>
+    <mergeCell ref="E86:E88"/>
+    <mergeCell ref="F86:F88"/>
+    <mergeCell ref="G86:G88"/>
+    <mergeCell ref="H86:H88"/>
+    <mergeCell ref="J86:J88"/>
+    <mergeCell ref="E69:E72"/>
+    <mergeCell ref="F69:F72"/>
+    <mergeCell ref="E74:E77"/>
+    <mergeCell ref="F74:F77"/>
+    <mergeCell ref="G74:G77"/>
+    <mergeCell ref="H74:H77"/>
+    <mergeCell ref="J74:J77"/>
+    <mergeCell ref="D74:D77"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -3426,7 +3428,7 @@
   </sheetPr>
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -3442,7 +3444,7 @@
     <col min="8" max="8" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" ht="13.8">
       <c r="A1" s="27" t="s">
         <v>77</v>
       </c>
@@ -3528,7 +3530,7 @@
       <c r="K5" s="31"/>
       <c r="L5" s="31"/>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" ht="13.8">
       <c r="A6" s="55"/>
       <c r="B6" s="44"/>
       <c r="C6" s="44"/>
@@ -3641,7 +3643,7 @@
       <c r="K12" s="31"/>
       <c r="L12" s="31"/>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" ht="13.8">
       <c r="A13" s="55"/>
       <c r="B13" s="44"/>
       <c r="C13" s="44"/>
@@ -3655,7 +3657,7 @@
       <c r="K13" s="31"/>
       <c r="L13" s="31"/>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" ht="55.2">
       <c r="A14" s="34" t="s">
         <v>98</v>
       </c>
@@ -3673,7 +3675,7 @@
       <c r="K14" s="31"/>
       <c r="L14" s="31"/>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" ht="27.6">
       <c r="A15" s="34" t="s">
         <v>100</v>
       </c>
@@ -3691,7 +3693,7 @@
       <c r="K15" s="31"/>
       <c r="L15" s="31"/>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" ht="41.4">
       <c r="A16" s="36"/>
       <c r="B16" s="29"/>
       <c r="C16" s="29"/>
@@ -3707,7 +3709,7 @@
       <c r="K16" s="31"/>
       <c r="L16" s="31"/>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" ht="41.4">
       <c r="A17" s="36"/>
       <c r="B17" s="29"/>
       <c r="C17" s="29"/>
@@ -3723,7 +3725,7 @@
       <c r="K17" s="31"/>
       <c r="L17" s="31"/>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" ht="13.8">
       <c r="A18" s="55"/>
       <c r="B18" s="44"/>
       <c r="C18" s="44"/>
@@ -3737,7 +3739,7 @@
       <c r="K18" s="31"/>
       <c r="L18" s="31"/>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" ht="69">
       <c r="A19" s="34" t="s">
         <v>104</v>
       </c>
@@ -3755,7 +3757,7 @@
       <c r="K19" s="31"/>
       <c r="L19" s="31"/>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" ht="41.4">
       <c r="A20" s="34" t="s">
         <v>106</v>
       </c>
@@ -3773,7 +3775,7 @@
       <c r="K20" s="31"/>
       <c r="L20" s="31"/>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" ht="41.4">
       <c r="B21" s="29"/>
       <c r="C21" s="29"/>
       <c r="D21" s="29"/>
@@ -3788,7 +3790,7 @@
       <c r="K21" s="31"/>
       <c r="L21" s="31"/>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" ht="55.2">
       <c r="A22" s="29"/>
       <c r="B22" s="29"/>
       <c r="C22" s="29"/>
@@ -3804,7 +3806,7 @@
       <c r="K22" s="31"/>
       <c r="L22" s="31"/>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" ht="55.2">
       <c r="A23" s="29"/>
       <c r="B23" s="29"/>
       <c r="C23" s="29"/>
@@ -3820,7 +3822,7 @@
       <c r="K23" s="31"/>
       <c r="L23" s="31"/>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" ht="13.8">
       <c r="A24" s="55"/>
       <c r="B24" s="44"/>
       <c r="C24" s="44"/>
@@ -3834,7 +3836,7 @@
       <c r="K24" s="31"/>
       <c r="L24" s="31"/>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" ht="55.2">
       <c r="A25" s="34" t="s">
         <v>111</v>
       </c>
@@ -3852,7 +3854,7 @@
       <c r="K25" s="31"/>
       <c r="L25" s="31"/>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" ht="69">
       <c r="A26" s="34" t="s">
         <v>113</v>
       </c>
@@ -3870,7 +3872,7 @@
       <c r="K26" s="31"/>
       <c r="L26" s="31"/>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" ht="82.8">
       <c r="B27" s="29"/>
       <c r="C27" s="29"/>
       <c r="D27" s="29"/>
@@ -3885,7 +3887,7 @@
       <c r="K27" s="31"/>
       <c r="L27" s="31"/>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" ht="13.8">
       <c r="A28" s="32"/>
       <c r="B28" s="38"/>
       <c r="C28" s="38"/>
@@ -3894,7 +3896,7 @@
       <c r="F28" s="56"/>
       <c r="G28" s="45"/>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" ht="96.6">
       <c r="A29" s="34" t="s">
         <v>116</v>
       </c>
@@ -3907,7 +3909,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" ht="13.8">
       <c r="A30" s="34" t="s">
         <v>118</v>
       </c>
@@ -3918,7 +3920,7 @@
       <c r="F30" s="29"/>
       <c r="G30" s="37"/>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" ht="13.8">
       <c r="A31" s="55"/>
       <c r="B31" s="44"/>
       <c r="C31" s="44"/>

</xml_diff>

<commit_message>
Actualizacion Carpeta Documentacion 10
</commit_message>
<xml_diff>
--- a/Documentacion/Backlog ,Sprints, Story Mapping/6.0Backlog, Sprints, Story Mapping.xlsx
+++ b/Documentacion/Backlog ,Sprints, Story Mapping/6.0Backlog, Sprints, Story Mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcben\OneDrive\Escritorio\Proyecto-Software-I\Documentacion\Backlog ,Sprints, Story Mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFE6F275-E122-41B6-B35A-372ED19BD460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A3B6753-CC1D-44F5-8884-2EEC69C163E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -724,24 +724,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -998,8 +998,8 @@
   </sheetPr>
   <dimension ref="D5:P24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H12" zoomScale="86" workbookViewId="0">
-      <selection activeCell="S15" sqref="S15"/>
+    <sheetView tabSelected="1" topLeftCell="I9" zoomScale="86" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1"/>
@@ -1150,7 +1150,7 @@
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
     </row>
-    <row r="13" spans="4:16" ht="57.6">
+    <row r="13" spans="4:16" ht="72">
       <c r="D13" s="5">
         <v>3</v>
       </c>
@@ -1166,20 +1166,20 @@
       <c r="H13" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="L13" s="1">
+      <c r="L13" s="5">
         <v>3</v>
       </c>
-      <c r="M13" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="N13" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="O13" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="P13" s="2" t="s">
-        <v>21</v>
+      <c r="M13" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="N13" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="O13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="P13" s="6" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="4:16" ht="14.4">
@@ -1210,20 +1210,20 @@
       <c r="H15" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L15" s="5">
+      <c r="L15" s="1">
         <v>4</v>
       </c>
-      <c r="M15" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="N15" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="O15" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="P15" s="6" t="s">
-        <v>14</v>
+      <c r="M15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O15" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="P15" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="4:16" ht="12.75" customHeight="1">
@@ -1836,11 +1836,11 @@
     </row>
     <row r="51" spans="4:16" ht="18" customHeight="1"/>
     <row r="53" spans="4:16" ht="18" customHeight="1">
-      <c r="J53" s="49"/>
-      <c r="K53" s="49"/>
-      <c r="L53" s="49"/>
-      <c r="M53" s="49"/>
-      <c r="N53" s="49"/>
+      <c r="J53" s="52"/>
+      <c r="K53" s="52"/>
+      <c r="L53" s="52"/>
+      <c r="M53" s="52"/>
+      <c r="N53" s="52"/>
     </row>
     <row r="54" spans="4:16" ht="18" customHeight="1">
       <c r="D54" s="11"/>
@@ -1879,7 +1879,7 @@
       <c r="H56" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="J56" s="48" t="s">
+      <c r="J56" s="49" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1923,7 +1923,7 @@
       <c r="H60" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="J60" s="48" t="s">
+      <c r="J60" s="49" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1975,7 +1975,7 @@
       <c r="H65" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="J65" s="48" t="s">
+      <c r="J65" s="49" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2013,13 +2013,13 @@
       <c r="F69" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="G69" s="54" t="s">
+      <c r="G69" s="48" t="s">
         <v>45</v>
       </c>
       <c r="H69" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="J69" s="48" t="s">
+      <c r="J69" s="49" t="s">
         <v>65</v>
       </c>
     </row>
@@ -2068,10 +2068,10 @@
       <c r="G74" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="H74" s="54" t="s">
+      <c r="H74" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="J74" s="48" t="s">
+      <c r="J74" s="49" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2173,13 +2173,13 @@
       <c r="F83" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="G83" s="54" t="s">
+      <c r="G83" s="48" t="s">
         <v>38</v>
       </c>
       <c r="H83" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="J83" s="48" t="s">
+      <c r="J83" s="49" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2215,7 +2215,7 @@
       <c r="H86" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="J86" s="48" t="s">
+      <c r="J86" s="49" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2287,7 +2287,7 @@
       <c r="H92" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="J92" s="48" t="s">
+      <c r="J92" s="49" t="s">
         <v>75</v>
       </c>
     </row>
@@ -2339,7 +2339,7 @@
       <c r="H97" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="J97" s="48" t="s">
+      <c r="J97" s="49" t="s">
         <v>76</v>
       </c>
     </row>
@@ -2377,27 +2377,27 @@
     </row>
     <row r="102" spans="4:13" ht="18" customHeight="1">
       <c r="D102" s="51"/>
-      <c r="E102" s="52"/>
-      <c r="F102" s="52"/>
-      <c r="G102" s="52"/>
-      <c r="H102" s="52"/>
-      <c r="J102" s="53"/>
+      <c r="E102" s="53"/>
+      <c r="F102" s="53"/>
+      <c r="G102" s="53"/>
+      <c r="H102" s="53"/>
+      <c r="J102" s="54"/>
     </row>
     <row r="103" spans="4:13" ht="18" customHeight="1">
-      <c r="D103" s="49"/>
-      <c r="E103" s="49"/>
-      <c r="F103" s="49"/>
-      <c r="G103" s="49"/>
-      <c r="H103" s="49"/>
-      <c r="J103" s="49"/>
+      <c r="D103" s="52"/>
+      <c r="E103" s="52"/>
+      <c r="F103" s="52"/>
+      <c r="G103" s="52"/>
+      <c r="H103" s="52"/>
+      <c r="J103" s="52"/>
     </row>
     <row r="104" spans="4:13" ht="18" customHeight="1">
-      <c r="D104" s="49"/>
-      <c r="E104" s="49"/>
-      <c r="F104" s="49"/>
-      <c r="G104" s="49"/>
-      <c r="H104" s="49"/>
-      <c r="J104" s="49"/>
+      <c r="D104" s="52"/>
+      <c r="E104" s="52"/>
+      <c r="F104" s="52"/>
+      <c r="G104" s="52"/>
+      <c r="H104" s="52"/>
+      <c r="J104" s="52"/>
       <c r="M104" s="26"/>
     </row>
     <row r="105" spans="4:13" ht="18" customHeight="1"/>
@@ -3300,95 +3300,6 @@
     <row r="1002" ht="18" customHeight="1"/>
   </sheetData>
   <mergeCells count="113">
-    <mergeCell ref="G9:G12"/>
-    <mergeCell ref="H9:H12"/>
-    <mergeCell ref="D3:H3"/>
-    <mergeCell ref="D4:D7"/>
-    <mergeCell ref="E4:E7"/>
-    <mergeCell ref="F4:F7"/>
-    <mergeCell ref="G4:G7"/>
-    <mergeCell ref="H4:H7"/>
-    <mergeCell ref="D9:D12"/>
-    <mergeCell ref="E9:E12"/>
-    <mergeCell ref="F9:F12"/>
-    <mergeCell ref="D16:D19"/>
-    <mergeCell ref="E16:E19"/>
-    <mergeCell ref="F16:F19"/>
-    <mergeCell ref="G16:G19"/>
-    <mergeCell ref="H16:H19"/>
-    <mergeCell ref="F24:F26"/>
-    <mergeCell ref="G24:G26"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="H21:H22"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="H24:H26"/>
-    <mergeCell ref="D24:D26"/>
-    <mergeCell ref="D83:D84"/>
-    <mergeCell ref="E83:E84"/>
-    <mergeCell ref="F83:F84"/>
-    <mergeCell ref="G83:G84"/>
-    <mergeCell ref="H83:H84"/>
-    <mergeCell ref="J83:J84"/>
-    <mergeCell ref="G69:G72"/>
-    <mergeCell ref="H69:H72"/>
-    <mergeCell ref="G33:G35"/>
-    <mergeCell ref="H33:H35"/>
-    <mergeCell ref="F47:F49"/>
-    <mergeCell ref="G47:G49"/>
-    <mergeCell ref="D43:D45"/>
-    <mergeCell ref="E43:E45"/>
-    <mergeCell ref="F43:F45"/>
-    <mergeCell ref="G43:G45"/>
-    <mergeCell ref="H43:H45"/>
-    <mergeCell ref="D47:D49"/>
-    <mergeCell ref="E47:E49"/>
-    <mergeCell ref="H47:H49"/>
-    <mergeCell ref="D102:D104"/>
-    <mergeCell ref="E102:E104"/>
-    <mergeCell ref="F102:F104"/>
-    <mergeCell ref="G102:G104"/>
-    <mergeCell ref="H102:H104"/>
-    <mergeCell ref="J102:J104"/>
-    <mergeCell ref="D92:D95"/>
-    <mergeCell ref="D97:D100"/>
-    <mergeCell ref="E97:E100"/>
-    <mergeCell ref="F97:F100"/>
-    <mergeCell ref="G97:G100"/>
-    <mergeCell ref="H97:H100"/>
-    <mergeCell ref="J97:J100"/>
-    <mergeCell ref="G92:G95"/>
-    <mergeCell ref="H92:H95"/>
-    <mergeCell ref="J92:J95"/>
-    <mergeCell ref="D28:D31"/>
-    <mergeCell ref="E28:E31"/>
-    <mergeCell ref="F28:F31"/>
-    <mergeCell ref="G28:G31"/>
-    <mergeCell ref="H28:H31"/>
-    <mergeCell ref="D33:D35"/>
-    <mergeCell ref="E33:E35"/>
-    <mergeCell ref="F33:F35"/>
-    <mergeCell ref="D39:D41"/>
-    <mergeCell ref="E39:E41"/>
-    <mergeCell ref="F39:F41"/>
-    <mergeCell ref="G39:G41"/>
-    <mergeCell ref="H39:H41"/>
-    <mergeCell ref="J53:N53"/>
-    <mergeCell ref="D55:H55"/>
-    <mergeCell ref="E56:E58"/>
-    <mergeCell ref="F56:F58"/>
-    <mergeCell ref="G56:G58"/>
-    <mergeCell ref="H56:H58"/>
-    <mergeCell ref="J56:J58"/>
-    <mergeCell ref="D56:D58"/>
-    <mergeCell ref="D60:D63"/>
-    <mergeCell ref="E60:E63"/>
-    <mergeCell ref="F60:F63"/>
-    <mergeCell ref="G60:G63"/>
-    <mergeCell ref="H60:H63"/>
-    <mergeCell ref="J60:J63"/>
     <mergeCell ref="D65:D67"/>
     <mergeCell ref="E65:E67"/>
     <mergeCell ref="F65:F67"/>
@@ -3413,6 +3324,95 @@
     <mergeCell ref="H74:H77"/>
     <mergeCell ref="J74:J77"/>
     <mergeCell ref="D74:D77"/>
+    <mergeCell ref="G56:G58"/>
+    <mergeCell ref="H56:H58"/>
+    <mergeCell ref="J56:J58"/>
+    <mergeCell ref="D56:D58"/>
+    <mergeCell ref="D60:D63"/>
+    <mergeCell ref="E60:E63"/>
+    <mergeCell ref="F60:F63"/>
+    <mergeCell ref="G60:G63"/>
+    <mergeCell ref="H60:H63"/>
+    <mergeCell ref="J60:J63"/>
+    <mergeCell ref="D28:D31"/>
+    <mergeCell ref="E28:E31"/>
+    <mergeCell ref="F28:F31"/>
+    <mergeCell ref="G28:G31"/>
+    <mergeCell ref="H28:H31"/>
+    <mergeCell ref="D33:D35"/>
+    <mergeCell ref="E33:E35"/>
+    <mergeCell ref="F33:F35"/>
+    <mergeCell ref="D39:D41"/>
+    <mergeCell ref="E39:E41"/>
+    <mergeCell ref="F39:F41"/>
+    <mergeCell ref="G39:G41"/>
+    <mergeCell ref="H39:H41"/>
+    <mergeCell ref="D102:D104"/>
+    <mergeCell ref="E102:E104"/>
+    <mergeCell ref="F102:F104"/>
+    <mergeCell ref="G102:G104"/>
+    <mergeCell ref="H102:H104"/>
+    <mergeCell ref="J102:J104"/>
+    <mergeCell ref="D92:D95"/>
+    <mergeCell ref="D97:D100"/>
+    <mergeCell ref="E97:E100"/>
+    <mergeCell ref="F97:F100"/>
+    <mergeCell ref="G97:G100"/>
+    <mergeCell ref="H97:H100"/>
+    <mergeCell ref="J97:J100"/>
+    <mergeCell ref="G92:G95"/>
+    <mergeCell ref="H92:H95"/>
+    <mergeCell ref="J92:J95"/>
+    <mergeCell ref="D83:D84"/>
+    <mergeCell ref="E83:E84"/>
+    <mergeCell ref="F83:F84"/>
+    <mergeCell ref="G83:G84"/>
+    <mergeCell ref="H83:H84"/>
+    <mergeCell ref="J83:J84"/>
+    <mergeCell ref="G69:G72"/>
+    <mergeCell ref="H69:H72"/>
+    <mergeCell ref="G33:G35"/>
+    <mergeCell ref="H33:H35"/>
+    <mergeCell ref="F47:F49"/>
+    <mergeCell ref="G47:G49"/>
+    <mergeCell ref="D43:D45"/>
+    <mergeCell ref="E43:E45"/>
+    <mergeCell ref="F43:F45"/>
+    <mergeCell ref="G43:G45"/>
+    <mergeCell ref="H43:H45"/>
+    <mergeCell ref="D47:D49"/>
+    <mergeCell ref="E47:E49"/>
+    <mergeCell ref="H47:H49"/>
+    <mergeCell ref="J53:N53"/>
+    <mergeCell ref="D55:H55"/>
+    <mergeCell ref="E56:E58"/>
+    <mergeCell ref="F56:F58"/>
+    <mergeCell ref="D16:D19"/>
+    <mergeCell ref="E16:E19"/>
+    <mergeCell ref="F16:F19"/>
+    <mergeCell ref="G16:G19"/>
+    <mergeCell ref="H16:H19"/>
+    <mergeCell ref="F24:F26"/>
+    <mergeCell ref="G24:G26"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="H21:H22"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="H24:H26"/>
+    <mergeCell ref="D24:D26"/>
+    <mergeCell ref="G9:G12"/>
+    <mergeCell ref="H9:H12"/>
+    <mergeCell ref="D3:H3"/>
+    <mergeCell ref="D4:D7"/>
+    <mergeCell ref="E4:E7"/>
+    <mergeCell ref="F4:F7"/>
+    <mergeCell ref="G4:G7"/>
+    <mergeCell ref="H4:H7"/>
+    <mergeCell ref="D9:D12"/>
+    <mergeCell ref="E9:E12"/>
+    <mergeCell ref="F9:F12"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>